<commit_message>
Highlight long company names (>17 characters)
</commit_message>
<xml_diff>
--- a/another_test.xlsx
+++ b/another_test.xlsx
@@ -52,12 +52,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -72,7 +78,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -81,6 +87,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -451,7 +463,7 @@
   <dimension ref="A1:N34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -749,9 +761,9 @@
           <t>Mohan</t>
         </is>
       </c>
-      <c r="C9" s="5" t="inlineStr">
-        <is>
-          <t>lyne.ai</t>
+      <c r="C9" s="6" t="inlineStr">
+        <is>
+          <t>lyne.aiaiodjoiwajdaiwdjawdi</t>
         </is>
       </c>
       <c r="D9" s="4" t="inlineStr">
@@ -1093,9 +1105,9 @@
           <t>Saeed</t>
         </is>
       </c>
-      <c r="C19" s="4" t="inlineStr">
-        <is>
-          <t>N/A</t>
+      <c r="C19" s="7" t="inlineStr">
+        <is>
+          <t>wadjaoiwdjawoidjawdijawdijawdoijawd</t>
         </is>
       </c>
       <c r="D19" s="4" t="inlineStr">
@@ -1373,9 +1385,9 @@
           <t>Saeed</t>
         </is>
       </c>
-      <c r="C29" s="4" t="inlineStr">
-        <is>
-          <t>N/A</t>
+      <c r="C29" s="7" t="inlineStr">
+        <is>
+          <t>N/Awaoidjajiadoijwadij</t>
         </is>
       </c>
       <c r="D29" s="4" t="inlineStr">

</xml_diff>